<commit_message>
Problems and allergies IHE compliant
</commit_message>
<xml_diff>
--- a/implementation/src/test/resouces/Dados TASY.xlsx
+++ b/implementation/src/test/resouces/Dados TASY.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Pacientes" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Resultados Laboratório" sheetId="19" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <webPublishing codePage="65001"/>
 </workbook>
 </file>
 
@@ -698,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -984,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD12"/>
     </sheetView>
   </sheetViews>

</xml_diff>